<commit_message>
add modelling for noised data and generating appropriate tables
</commit_message>
<xml_diff>
--- a/tables/resultsBackup.xlsx
+++ b/tables/resultsBackup.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16440" windowWidth="28110" xWindow="-27990" yWindow="-120"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modelling" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -422,8 +422,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="12.5703125"/>
-    <col bestFit="1" customWidth="1" max="5" min="2" width="12"/>
+    <col width="12.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12" bestFit="1" customWidth="1" min="2" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -687,7 +687,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -781,10 +781,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>329</v>
+        <v>346</v>
       </c>
       <c r="C3" t="n">
-        <v>328</v>
+        <v>345</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -792,10 +792,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="G3" t="n">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -803,10 +803,10 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>331</v>
+        <v>349</v>
       </c>
       <c r="K3" t="n">
-        <v>330</v>
+        <v>348</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="O3" t="n">
-        <v>328</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4119838681649083</v>
+        <v>0.9957368007414592</v>
       </c>
       <c r="C4" t="n">
-        <v>0.407991131274566</v>
+        <v>0.9957917657510439</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.451977465662363</v>
+        <v>0.9988934151795835</v>
       </c>
       <c r="G4" t="n">
-        <v>0.451977465662363</v>
+        <v>0.9988934151795835</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -849,10 +849,10 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0.3036957166024276</v>
+        <v>0.07456617805400845</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2992133488638447</v>
+        <v>0.07455375731348657</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -860,10 +860,10 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>0.3115245492574082</v>
+        <v>0.09473645879962589</v>
       </c>
       <c r="O4" t="n">
-        <v>0.3115245492574082</v>
+        <v>0.09473645879962589</v>
       </c>
     </row>
     <row r="5">
@@ -873,10 +873,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4522330541766292</v>
+        <v>0.995778058834679</v>
       </c>
       <c r="C5" t="n">
-        <v>0.448124527252474</v>
+        <v>0.995801635395351</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -884,10 +884,10 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.4712809044808305</v>
+        <v>0.9988651753657154</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4712809044808305</v>
+        <v>0.9988651753657154</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -895,10 +895,10 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0.33898090471995</v>
+        <v>0.07402426525385286</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3358350509716077</v>
+        <v>0.07389053541194934</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -906,10 +906,10 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>0.3428552741228628</v>
+        <v>0.09218837922826839</v>
       </c>
       <c r="O5" t="n">
-        <v>0.3428552741228628</v>
+        <v>0.09218837922826839</v>
       </c>
     </row>
     <row r="6">
@@ -919,10 +919,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.4921884167115415</v>
+        <v>0.9955987448874793</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4888234505398104</v>
+        <v>0.9956189769887136</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -930,10 +930,10 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.4975413980250909</v>
+        <v>0.9988722416207938</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4975413980250909</v>
+        <v>0.9988722416207938</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -941,10 +941,10 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0.3555080170867141</v>
+        <v>0.07466250097719018</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3565490917049647</v>
+        <v>0.07460929568291363</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="N6" t="n">
-        <v>0.3696074832313749</v>
+        <v>0.09063134454432165</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3696074832313749</v>
+        <v>0.09063134454432165</v>
       </c>
     </row>
     <row r="7">
@@ -965,10 +965,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.507948972017597</v>
+        <v>0.9949839145655118</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5077091916573608</v>
+        <v>0.9951115357807993</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -976,10 +976,10 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.4990317827415703</v>
+        <v>0.9988643044524392</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4990317827415703</v>
+        <v>0.9988643044524392</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -987,10 +987,10 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>0.3452091110769701</v>
+        <v>0.07305110945056126</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3468111116008235</v>
+        <v>0.07342755578251181</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
@@ -998,10 +998,10 @@
         </is>
       </c>
       <c r="N7" t="n">
-        <v>0.3776037580723052</v>
+        <v>0.08863230649054776</v>
       </c>
       <c r="O7" t="n">
-        <v>0.3776037580723052</v>
+        <v>0.08863230649054776</v>
       </c>
     </row>
     <row r="10">
@@ -1438,10 +1438,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C30" t="n">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1454,10 +1454,10 @@
         </is>
       </c>
       <c r="J30" t="n">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="K30" t="n">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="M30" t="inlineStr">
         <is>
@@ -1465,10 +1465,10 @@
         </is>
       </c>
       <c r="N30" t="n">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="O30" t="n">
-        <v>311</v>
+        <v>319</v>
       </c>
     </row>
     <row r="31">
@@ -1478,10 +1478,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3262101072361558</v>
+        <v>0.06866314750687252</v>
       </c>
       <c r="C31" t="n">
-        <v>0.3253536465400056</v>
+        <v>0.06826055285127608</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1494,10 +1494,10 @@
         </is>
       </c>
       <c r="J31" t="n">
-        <v>0.3113240440300592</v>
+        <v>0.06536514820025308</v>
       </c>
       <c r="K31" t="n">
-        <v>0.3107326883657398</v>
+        <v>0.06536514820025308</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
@@ -1505,10 +1505,10 @@
         </is>
       </c>
       <c r="N31" t="n">
-        <v>0.288347259902983</v>
+        <v>0.0739992422096668</v>
       </c>
       <c r="O31" t="n">
-        <v>0.288347259902983</v>
+        <v>0.0739992422096668</v>
       </c>
     </row>
     <row r="32">
@@ -1518,10 +1518,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.3410161550663044</v>
+        <v>0.07408269929472644</v>
       </c>
       <c r="C32" t="n">
-        <v>0.3388643415574109</v>
+        <v>0.07355318604759598</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1534,10 +1534,10 @@
         </is>
       </c>
       <c r="J32" t="n">
-        <v>0.3263667970350027</v>
+        <v>0.07042566275682982</v>
       </c>
       <c r="K32" t="n">
-        <v>0.3242630986448997</v>
+        <v>0.07042566275682982</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
@@ -1545,10 +1545,10 @@
         </is>
       </c>
       <c r="N32" t="n">
-        <v>0.3072059613997714</v>
+        <v>0.07901123518687858</v>
       </c>
       <c r="O32" t="n">
-        <v>0.3072059613997714</v>
+        <v>0.07901123518687858</v>
       </c>
     </row>
     <row r="33">
@@ -1558,10 +1558,10 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.3683137105285688</v>
+        <v>0.07699301677801429</v>
       </c>
       <c r="C33" t="n">
-        <v>0.3666587755050267</v>
+        <v>0.07674966343422662</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1574,10 +1574,10 @@
         </is>
       </c>
       <c r="J33" t="n">
-        <v>0.3532328831421846</v>
+        <v>0.07412178191509555</v>
       </c>
       <c r="K33" t="n">
-        <v>0.3507551528087574</v>
+        <v>0.07412178191509555</v>
       </c>
       <c r="M33" t="inlineStr">
         <is>
@@ -1585,10 +1585,10 @@
         </is>
       </c>
       <c r="N33" t="n">
-        <v>0.3290337435902809</v>
+        <v>0.08354979139152663</v>
       </c>
       <c r="O33" t="n">
-        <v>0.3290337435902809</v>
+        <v>0.08354979139152663</v>
       </c>
     </row>
     <row r="34">
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.3858569503928133</v>
+        <v>0.07643071499573506</v>
       </c>
       <c r="C34" t="n">
-        <v>0.3847030444517295</v>
+        <v>0.07666627330717168</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1614,10 +1614,10 @@
         </is>
       </c>
       <c r="J34" t="n">
-        <v>0.375385347969285</v>
+        <v>0.07477522465328801</v>
       </c>
       <c r="K34" t="n">
-        <v>0.3735426196500373</v>
+        <v>0.07477522465328801</v>
       </c>
       <c r="M34" t="inlineStr">
         <is>
@@ -1625,14 +1625,14 @@
         </is>
       </c>
       <c r="N34" t="n">
-        <v>0.3421768623701663</v>
+        <v>0.085980507366749</v>
       </c>
       <c r="O34" t="n">
-        <v>0.3421768623701663</v>
+        <v>0.085980507366749</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1726,10 +1726,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C3" t="n">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -1737,26 +1737,29 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="G3" t="n">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>Point of overcoming</t>
         </is>
       </c>
+      <c r="K3" t="n">
+        <v>350</v>
+      </c>
       <c r="M3" t="inlineStr">
         <is>
           <t>Point of overcoming</t>
         </is>
       </c>
       <c r="N3" t="n">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="O3" t="n">
-        <v>338</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4">
@@ -1766,10 +1769,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1722369229848595</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1726458259821523</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -1777,15 +1780,18 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.1727774732282191</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1727774732282191</v>
+        <v>1</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
           <t>X[point]</t>
         </is>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -1806,10 +1812,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1724268726985223</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1728176641611908</v>
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -1817,15 +1823,18 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.172777473228219</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.172777473228219</v>
+        <v>1</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>X[point+10]</t>
         </is>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -1846,10 +1855,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1726458259821589</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1728824878416787</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1857,15 +1866,18 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.1727774732282187</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1727774732282187</v>
+        <v>1</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
           <t>X[point+20]</t>
         </is>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -1886,10 +1898,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1728176641611981</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1728176641611975</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1897,15 +1909,18 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.1727774732282188</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1727774732282188</v>
+        <v>1</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
           <t>X[point+30]</t>
         </is>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
@@ -2547,6 +2562,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>